<commit_message>
Reran calculations (should be no change in result) and updated the evolutions figure.
</commit_message>
<xml_diff>
--- a/Trudgill_et_al_202X/Data/TJ_d11B_pH.xlsx
+++ b/Trudgill_et_al_202X/Data/TJ_d11B_pH.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
   <si>
     <t>sample</t>
   </si>
@@ -350,6 +350,33 @@
   </si>
   <si>
     <t>Ma</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>°C</t>
   </si>
 </sst>
 </file>
@@ -373,7 +400,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -408,11 +435,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -441,6 +471,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,28 +830,28 @@
         <v>102</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.3">
@@ -838,28 +871,28 @@
         <v>104</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.3">

</xml_diff>